<commit_message>
Gate Entry Page added
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharb\eclipse-workspace\WM\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6964B21-D5DE-492C-AF84-1471520520EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2FD115-109F-4B98-BEC0-828FA187A66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{19E298D3-9C1F-4AA6-B873-7A34EC87055D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Data1" sheetId="2" r:id="rId2"/>
-    <sheet name="Data2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TestCases</t>
   </si>
@@ -53,44 +52,56 @@
     <t>Bcil@12345678</t>
   </si>
   <si>
-    <t>Bcil@987654321</t>
-  </si>
-  <si>
-    <t>TestCase002-Valid user name and invalid password.</t>
-  </si>
-  <si>
-    <t>TestCase001- Valid user name and password.</t>
-  </si>
-  <si>
-    <t>resp</t>
-  </si>
-  <si>
-    <t>©2025-2026 Bar Code India Limited. All rights reserved.</t>
-  </si>
-  <si>
-    <t>Invalid username or password!</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
     <t>Positive</t>
   </si>
   <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>qwer</t>
-  </si>
-  <si>
-    <t>TestCase003-Valid user name and invalid password.</t>
+    <t>docType</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>TestCase001- Gate Entry with the Complete Qty receiving of all the material codes from the selected order.</t>
+  </si>
+  <si>
+    <t>documentNo</t>
+  </si>
+  <si>
+    <t>TNTINV8910</t>
+  </si>
+  <si>
+    <t>invoiceNum</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>vehicleNum</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>24-052025</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>DL8SQQ7313</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,11 +114,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,7 +138,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,88 +455,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC65D3E-B736-4688-B869-19C25D491A82}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="J2" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.3984375" customWidth="1"/>
-    <col min="3" max="3" width="29.265625" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" customWidth="1"/>
-    <col min="5" max="5" width="56.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.06640625" style="1"/>
+    <col min="8" max="8" width="4.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.06640625" style="1"/>
+    <col min="11" max="11" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>24032502</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1">
+        <v>9999999999</v>
       </c>
     </row>
   </sheetData>
@@ -536,36 +550,8 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="nikhil.kharb@ymail.com" xr:uid="{8CCC1BFE-A980-4870-8A76-9810E07A3325}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{B41FB479-8A01-4483-AD68-A1676A6F4D70}"/>
-    <hyperlink ref="C3" r:id="rId3" display="nikfhil@rmail.com" xr:uid="{6C6631EC-9899-42A3-9F76-92622C1C964B}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{BBAFDC6C-A00E-4C33-A52E-92713BBC5E6D}"/>
-    <hyperlink ref="C4" r:id="rId5" display="nikfhil@rmail.com" xr:uid="{BDCD7310-086C-49D1-AAE7-5501A71AEE69}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{833A387E-8344-4683-BC3E-0D9895EEAAC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D68306-8BE0-402F-8F39-522AFEF78067}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44D6AA5-7E2D-4CD7-97BD-D68F663C59DB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>